<commit_message>
dashboard almost ready: make second worksheet for Yulia and load previous results
</commit_message>
<xml_diff>
--- a/templates/programs.xlsx
+++ b/templates/programs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tijuanap\Programs\HSE_dashboard\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/iasonov/Programming/Python/HSE_dashboard/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF8CE698-6ABD-4ABE-B691-348A4C51B6B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA7389B3-0AF7-BA45-8B59-8075E4564235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{459C6DFD-26EB-1040-9D7C-59DC53018D97}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16460" xr2:uid="{459C6DFD-26EB-1040-9D7C-59DC53018D97}"/>
   </bookViews>
   <sheets>
     <sheet name="programs" sheetId="1" r:id="rId1"/>
@@ -634,9 +634,6 @@
     <t>Цифровая инженерия для компьютерных игр</t>
   </si>
   <si>
-    <t>Управление бизнесом (бак), Пермь</t>
-  </si>
-  <si>
     <t>Биоинформатика в агробиотехнологиях</t>
   </si>
   <si>
@@ -700,9 +697,6 @@
     <t>КИБЕРБЕЗ. Кибербезопасность / Москва / 100401 Информационная безопасность / Московский институт электроники и математики им АН Тихонова / Магистратура</t>
   </si>
   <si>
-    <t>КИТЯЗ. Китайский язык в межкультурной бизнескоммуникации / Москва / 450402 Лингвистика / Школа иностранных языков / Магистратура</t>
-  </si>
-  <si>
     <t>КНАД. Компьютерные науки и анализ данных / Москва / 010302 Прикладная математика и информатика / факультет компьютерных наук / Бакалавриат</t>
   </si>
   <si>
@@ -779,6 +773,12 @@
   </si>
   <si>
     <t>plan_state</t>
+  </si>
+  <si>
+    <t>Управление бизнесом - онлайн (О К)</t>
+  </si>
+  <si>
+    <t>КИТЯЗ. Китайский язык в межкультурной бизнес-коммуникации.</t>
   </si>
 </sst>
 </file>
@@ -850,16 +850,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -878,9 +873,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -918,7 +913,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1024,7 +1019,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1166,7 +1161,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1177,20 +1172,20 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:I194"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31:F194"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="150" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I77" sqref="I77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.875" customWidth="1"/>
-    <col min="2" max="2" width="8.125" customWidth="1"/>
-    <col min="3" max="6" width="7.625" customWidth="1"/>
+    <col min="1" max="1" width="35.83203125" customWidth="1"/>
+    <col min="2" max="2" width="8.1640625" customWidth="1"/>
+    <col min="3" max="6" width="7.6640625" customWidth="1"/>
     <col min="8" max="8" width="6" customWidth="1"/>
     <col min="9" max="9" width="46" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>185</v>
       </c>
@@ -1200,26 +1195,26 @@
       <c r="C1" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>246</v>
+      <c r="D1" t="s">
+        <v>244</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>186</v>
       </c>
       <c r="H1" t="s">
+        <v>203</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>183</v>
       </c>
@@ -1235,7 +1230,7 @@
       </c>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>182</v>
       </c>
@@ -1251,7 +1246,7 @@
       </c>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>181</v>
       </c>
@@ -1267,7 +1262,7 @@
       </c>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>180</v>
       </c>
@@ -1283,7 +1278,7 @@
       </c>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>179</v>
       </c>
@@ -1299,7 +1294,7 @@
       </c>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>178</v>
       </c>
@@ -1315,7 +1310,7 @@
       </c>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>177</v>
       </c>
@@ -1341,10 +1336,10 @@
         <v>50</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>176</v>
       </c>
@@ -1360,7 +1355,7 @@
       </c>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>175</v>
       </c>
@@ -1386,10 +1381,10 @@
         <v>100</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>174</v>
       </c>
@@ -1405,7 +1400,7 @@
       </c>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>173</v>
       </c>
@@ -1421,7 +1416,7 @@
       </c>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>172</v>
       </c>
@@ -1437,7 +1432,7 @@
       </c>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>171</v>
       </c>
@@ -1453,7 +1448,7 @@
       </c>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>170</v>
       </c>
@@ -1469,7 +1464,7 @@
       </c>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>169</v>
       </c>
@@ -1485,7 +1480,7 @@
       </c>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>168</v>
       </c>
@@ -1501,7 +1496,7 @@
       </c>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>167</v>
       </c>
@@ -1517,7 +1512,7 @@
       </c>
       <c r="H18" s="1"/>
     </row>
-    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>166</v>
       </c>
@@ -1533,7 +1528,7 @@
       </c>
       <c r="H19" s="1"/>
     </row>
-    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>165</v>
       </c>
@@ -1549,7 +1544,7 @@
       </c>
       <c r="H20" s="1"/>
     </row>
-    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>164</v>
       </c>
@@ -1565,7 +1560,7 @@
       </c>
       <c r="H21" s="1"/>
     </row>
-    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>163</v>
       </c>
@@ -1581,7 +1576,7 @@
       </c>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>162</v>
       </c>
@@ -1597,7 +1592,7 @@
       </c>
       <c r="H23" s="1"/>
     </row>
-    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>161</v>
       </c>
@@ -1613,7 +1608,7 @@
       </c>
       <c r="H24" s="1"/>
     </row>
-    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>160</v>
       </c>
@@ -1629,7 +1624,7 @@
       </c>
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>159</v>
       </c>
@@ -1645,7 +1640,7 @@
       </c>
       <c r="H26" s="1"/>
     </row>
-    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>158</v>
       </c>
@@ -1661,7 +1656,7 @@
       </c>
       <c r="H27" s="1"/>
     </row>
-    <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>157</v>
       </c>
@@ -1677,7 +1672,7 @@
       </c>
       <c r="H28" s="1"/>
     </row>
-    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>156</v>
       </c>
@@ -1693,36 +1688,36 @@
       </c>
       <c r="H29" s="1"/>
     </row>
-    <row r="30" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
-        <v>199</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C30" s="5">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>198</v>
+      </c>
+      <c r="B30" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30">
         <v>490</v>
       </c>
-      <c r="D30" s="6">
+      <c r="D30" s="1">
         <v>15</v>
       </c>
-      <c r="E30" s="5">
+      <c r="E30">
         <v>15</v>
       </c>
-      <c r="F30" s="5">
-        <v>0</v>
-      </c>
-      <c r="G30" s="5" t="s">
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30" t="s">
         <v>72</v>
       </c>
-      <c r="H30" s="5">
+      <c r="H30">
         <v>100</v>
       </c>
-      <c r="I30" s="7" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I30" s="2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>187</v>
       </c>
@@ -1748,10 +1743,10 @@
         <v>100</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>153</v>
       </c>
@@ -1767,7 +1762,7 @@
       </c>
       <c r="H32" s="1"/>
     </row>
-    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>152</v>
       </c>
@@ -1783,7 +1778,7 @@
       </c>
       <c r="H33" s="1"/>
     </row>
-    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>151</v>
       </c>
@@ -1799,7 +1794,7 @@
       </c>
       <c r="H34" s="1"/>
     </row>
-    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>150</v>
       </c>
@@ -1815,7 +1810,7 @@
       </c>
       <c r="H35" s="1"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>188</v>
       </c>
@@ -1841,10 +1836,10 @@
         <v>100</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>148</v>
       </c>
@@ -1860,7 +1855,7 @@
       </c>
       <c r="H37" s="1"/>
     </row>
-    <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>147</v>
       </c>
@@ -1876,7 +1871,7 @@
       </c>
       <c r="H38" s="1"/>
     </row>
-    <row r="39" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>146</v>
       </c>
@@ -1892,7 +1887,7 @@
       </c>
       <c r="H39" s="1"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>189</v>
       </c>
@@ -1918,10 +1913,10 @@
         <v>100</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>155</v>
       </c>
@@ -1947,10 +1942,10 @@
         <v>100</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>154</v>
       </c>
@@ -1976,10 +1971,10 @@
         <v>50</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>142</v>
       </c>
@@ -1995,7 +1990,7 @@
       </c>
       <c r="H43" s="1"/>
     </row>
-    <row r="44" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>141</v>
       </c>
@@ -2011,7 +2006,7 @@
       </c>
       <c r="H44" s="1"/>
     </row>
-    <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>140</v>
       </c>
@@ -2027,7 +2022,7 @@
       </c>
       <c r="H45" s="1"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>149</v>
       </c>
@@ -2053,10 +2048,10 @@
         <v>100</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>145</v>
       </c>
@@ -2082,10 +2077,10 @@
         <v>100</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>137</v>
       </c>
@@ -2101,7 +2096,7 @@
       </c>
       <c r="H48" s="1"/>
     </row>
-    <row r="49" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>136</v>
       </c>
@@ -2117,7 +2112,7 @@
       </c>
       <c r="H49" s="1"/>
     </row>
-    <row r="50" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>135</v>
       </c>
@@ -2133,7 +2128,7 @@
       </c>
       <c r="H50" s="1"/>
     </row>
-    <row r="51" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>134</v>
       </c>
@@ -2149,7 +2144,7 @@
       </c>
       <c r="H51" s="1"/>
     </row>
-    <row r="52" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>133</v>
       </c>
@@ -2165,7 +2160,7 @@
       </c>
       <c r="H52" s="1"/>
     </row>
-    <row r="53" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>132</v>
       </c>
@@ -2188,7 +2183,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="54" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>131</v>
       </c>
@@ -2204,7 +2199,7 @@
       </c>
       <c r="H54" s="1"/>
     </row>
-    <row r="55" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>130</v>
       </c>
@@ -2220,7 +2215,7 @@
       </c>
       <c r="H55" s="1"/>
     </row>
-    <row r="56" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>129</v>
       </c>
@@ -2236,7 +2231,7 @@
       </c>
       <c r="H56" s="1"/>
     </row>
-    <row r="57" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>128</v>
       </c>
@@ -2252,7 +2247,7 @@
       </c>
       <c r="H57" s="1"/>
     </row>
-    <row r="58" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>127</v>
       </c>
@@ -2268,7 +2263,7 @@
       </c>
       <c r="H58" s="1"/>
     </row>
-    <row r="59" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>126</v>
       </c>
@@ -2284,7 +2279,7 @@
       </c>
       <c r="H59" s="1"/>
     </row>
-    <row r="60" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>125</v>
       </c>
@@ -2300,7 +2295,7 @@
       </c>
       <c r="H60" s="1"/>
     </row>
-    <row r="61" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>124</v>
       </c>
@@ -2316,7 +2311,7 @@
       </c>
       <c r="H61" s="1"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>144</v>
       </c>
@@ -2342,10 +2337,10 @@
         <v>100</v>
       </c>
       <c r="I62" s="2" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>122</v>
       </c>
@@ -2361,7 +2356,7 @@
       </c>
       <c r="H63" s="1"/>
     </row>
-    <row r="64" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>121</v>
       </c>
@@ -2377,7 +2372,7 @@
       </c>
       <c r="H64" s="1"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>143</v>
       </c>
@@ -2403,10 +2398,10 @@
         <v>100</v>
       </c>
       <c r="I65" s="2" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>139</v>
       </c>
@@ -2432,10 +2427,10 @@
         <v>100</v>
       </c>
       <c r="I66" s="2" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>118</v>
       </c>
@@ -2451,7 +2446,7 @@
       </c>
       <c r="H67" s="1"/>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>138</v>
       </c>
@@ -2477,10 +2472,10 @@
         <v>50</v>
       </c>
       <c r="I68" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>116</v>
       </c>
@@ -2496,7 +2491,7 @@
       </c>
       <c r="H69" s="1"/>
     </row>
-    <row r="70" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>115</v>
       </c>
@@ -2512,7 +2507,7 @@
       </c>
       <c r="H70" s="1"/>
     </row>
-    <row r="71" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>114</v>
       </c>
@@ -2528,7 +2523,7 @@
       </c>
       <c r="H71" s="1"/>
     </row>
-    <row r="72" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>113</v>
       </c>
@@ -2544,7 +2539,7 @@
       </c>
       <c r="H72" s="1"/>
     </row>
-    <row r="73" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>112</v>
       </c>
@@ -2560,7 +2555,7 @@
       </c>
       <c r="H73" s="1"/>
     </row>
-    <row r="74" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>111</v>
       </c>
@@ -2576,7 +2571,7 @@
       </c>
       <c r="H74" s="1"/>
     </row>
-    <row r="75" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>110</v>
       </c>
@@ -2592,7 +2587,7 @@
       </c>
       <c r="H75" s="1"/>
     </row>
-    <row r="76" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>109</v>
       </c>
@@ -2608,36 +2603,36 @@
       </c>
       <c r="H76" s="1"/>
     </row>
-    <row r="77" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="5" t="s">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
         <v>196</v>
       </c>
-      <c r="B77" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C77" s="5">
+      <c r="B77" t="s">
+        <v>0</v>
+      </c>
+      <c r="C77">
         <v>490</v>
       </c>
-      <c r="D77" s="6">
-        <v>0</v>
-      </c>
-      <c r="E77" s="5">
+      <c r="D77" s="1">
+        <v>0</v>
+      </c>
+      <c r="E77">
         <v>50</v>
       </c>
-      <c r="F77" s="5">
+      <c r="F77">
         <v>5</v>
       </c>
-      <c r="G77" s="5" t="s">
+      <c r="G77" t="s">
         <v>8</v>
       </c>
-      <c r="H77" s="5">
+      <c r="H77">
         <v>100</v>
       </c>
-      <c r="I77" s="7" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I77" s="2" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>107</v>
       </c>
@@ -2653,7 +2648,7 @@
       </c>
       <c r="H78" s="1"/>
     </row>
-    <row r="79" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>106</v>
       </c>
@@ -2669,7 +2664,7 @@
       </c>
       <c r="H79" s="1"/>
     </row>
-    <row r="80" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>105</v>
       </c>
@@ -2685,7 +2680,7 @@
       </c>
       <c r="H80" s="1"/>
     </row>
-    <row r="81" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>104</v>
       </c>
@@ -2701,7 +2696,7 @@
       </c>
       <c r="H81" s="1"/>
     </row>
-    <row r="82" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>103</v>
       </c>
@@ -2717,7 +2712,7 @@
       </c>
       <c r="H82" s="1"/>
     </row>
-    <row r="83" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>102</v>
       </c>
@@ -2733,7 +2728,7 @@
       </c>
       <c r="H83" s="1"/>
     </row>
-    <row r="84" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>101</v>
       </c>
@@ -2749,7 +2744,7 @@
       </c>
       <c r="H84" s="1"/>
     </row>
-    <row r="85" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>100</v>
       </c>
@@ -2765,7 +2760,7 @@
       </c>
       <c r="H85" s="1"/>
     </row>
-    <row r="86" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>99</v>
       </c>
@@ -2781,7 +2776,7 @@
       </c>
       <c r="H86" s="1"/>
     </row>
-    <row r="87" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>98</v>
       </c>
@@ -2797,7 +2792,7 @@
       </c>
       <c r="H87" s="1"/>
     </row>
-    <row r="88" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>97</v>
       </c>
@@ -2813,7 +2808,7 @@
       </c>
       <c r="H88" s="1"/>
     </row>
-    <row r="89" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>96</v>
       </c>
@@ -2829,7 +2824,7 @@
       </c>
       <c r="H89" s="1"/>
     </row>
-    <row r="90" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>95</v>
       </c>
@@ -2845,7 +2840,7 @@
       </c>
       <c r="H90" s="1"/>
     </row>
-    <row r="91" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>94</v>
       </c>
@@ -2861,7 +2856,7 @@
       </c>
       <c r="H91" s="1"/>
     </row>
-    <row r="92" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>93</v>
       </c>
@@ -2877,7 +2872,7 @@
       </c>
       <c r="H92" s="1"/>
     </row>
-    <row r="93" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>92</v>
       </c>
@@ -2893,7 +2888,7 @@
       </c>
       <c r="H93" s="1"/>
     </row>
-    <row r="94" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>91</v>
       </c>
@@ -2909,7 +2904,7 @@
       </c>
       <c r="H94" s="1"/>
     </row>
-    <row r="95" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>90</v>
       </c>
@@ -2925,7 +2920,7 @@
       </c>
       <c r="H95" s="1"/>
     </row>
-    <row r="96" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>89</v>
       </c>
@@ -2941,7 +2936,7 @@
       </c>
       <c r="H96" s="1"/>
     </row>
-    <row r="97" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>88</v>
       </c>
@@ -2957,7 +2952,7 @@
       </c>
       <c r="H97" s="1"/>
     </row>
-    <row r="98" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>87</v>
       </c>
@@ -2973,7 +2968,7 @@
       </c>
       <c r="H98" s="1"/>
     </row>
-    <row r="99" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>86</v>
       </c>
@@ -2989,7 +2984,7 @@
       </c>
       <c r="H99" s="1"/>
     </row>
-    <row r="100" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>85</v>
       </c>
@@ -3005,7 +3000,7 @@
       </c>
       <c r="H100" s="1"/>
     </row>
-    <row r="101" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>84</v>
       </c>
@@ -3021,7 +3016,7 @@
       </c>
       <c r="H101" s="1"/>
     </row>
-    <row r="102" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>83</v>
       </c>
@@ -3037,7 +3032,7 @@
       </c>
       <c r="H102" s="1"/>
     </row>
-    <row r="103" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>82</v>
       </c>
@@ -3053,7 +3048,7 @@
       </c>
       <c r="H103" s="1"/>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>190</v>
       </c>
@@ -3079,10 +3074,10 @@
         <v>100</v>
       </c>
       <c r="I104" s="2" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="105" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>80</v>
       </c>
@@ -3098,7 +3093,7 @@
       </c>
       <c r="H105" s="1"/>
     </row>
-    <row r="106" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>79</v>
       </c>
@@ -3114,7 +3109,7 @@
       </c>
       <c r="H106" s="1"/>
     </row>
-    <row r="107" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>78</v>
       </c>
@@ -3130,7 +3125,7 @@
       </c>
       <c r="H107" s="1"/>
     </row>
-    <row r="108" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>77</v>
       </c>
@@ -3146,7 +3141,7 @@
       </c>
       <c r="H108" s="1"/>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>123</v>
       </c>
@@ -3172,10 +3167,10 @@
         <v>50</v>
       </c>
       <c r="I109" s="2" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="110" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>75</v>
       </c>
@@ -3191,7 +3186,7 @@
       </c>
       <c r="H110" s="1"/>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>120</v>
       </c>
@@ -3217,10 +3212,10 @@
         <v>100</v>
       </c>
       <c r="I111" s="2" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
         <v>119</v>
       </c>
@@ -3246,10 +3241,10 @@
         <v>100</v>
       </c>
       <c r="I112" s="2" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="113" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
         <v>71</v>
       </c>
@@ -3265,7 +3260,7 @@
       </c>
       <c r="H113" s="1"/>
     </row>
-    <row r="114" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
         <v>70</v>
       </c>
@@ -3281,7 +3276,7 @@
       </c>
       <c r="H114" s="1"/>
     </row>
-    <row r="115" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
         <v>69</v>
       </c>
@@ -3297,7 +3292,7 @@
       </c>
       <c r="H115" s="1"/>
     </row>
-    <row r="116" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>68</v>
       </c>
@@ -3313,7 +3308,7 @@
       </c>
       <c r="H116" s="1"/>
     </row>
-    <row r="117" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>67</v>
       </c>
@@ -3329,7 +3324,7 @@
       </c>
       <c r="H117" s="1"/>
     </row>
-    <row r="118" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>66</v>
       </c>
@@ -3345,7 +3340,7 @@
       </c>
       <c r="H118" s="1"/>
     </row>
-    <row r="119" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
         <v>65</v>
       </c>
@@ -3361,7 +3356,7 @@
       </c>
       <c r="H119" s="1"/>
     </row>
-    <row r="120" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>64</v>
       </c>
@@ -3377,7 +3372,7 @@
       </c>
       <c r="H120" s="1"/>
     </row>
-    <row r="121" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
         <v>63</v>
       </c>
@@ -3393,7 +3388,7 @@
       </c>
       <c r="H121" s="1"/>
     </row>
-    <row r="122" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
         <v>62</v>
       </c>
@@ -3409,7 +3404,7 @@
       </c>
       <c r="H122" s="1"/>
     </row>
-    <row r="123" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
         <v>61</v>
       </c>
@@ -3425,7 +3420,7 @@
       </c>
       <c r="H123" s="1"/>
     </row>
-    <row r="124" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
         <v>60</v>
       </c>
@@ -3441,7 +3436,7 @@
       </c>
       <c r="H124" s="1"/>
     </row>
-    <row r="125" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>59</v>
       </c>
@@ -3457,7 +3452,7 @@
       </c>
       <c r="H125" s="1"/>
     </row>
-    <row r="126" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
         <v>58</v>
       </c>
@@ -3473,7 +3468,7 @@
       </c>
       <c r="H126" s="1"/>
     </row>
-    <row r="127" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
         <v>57</v>
       </c>
@@ -3489,7 +3484,7 @@
       </c>
       <c r="H127" s="1"/>
     </row>
-    <row r="128" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
         <v>56</v>
       </c>
@@ -3505,7 +3500,7 @@
       </c>
       <c r="H128" s="1"/>
     </row>
-    <row r="129" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
         <v>55</v>
       </c>
@@ -3521,7 +3516,7 @@
       </c>
       <c r="H129" s="1"/>
     </row>
-    <row r="130" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
         <v>54</v>
       </c>
@@ -3537,7 +3532,7 @@
       </c>
       <c r="H130" s="1"/>
     </row>
-    <row r="131" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
         <v>53</v>
       </c>
@@ -3553,7 +3548,7 @@
       </c>
       <c r="H131" s="1"/>
     </row>
-    <row r="132" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
         <v>52</v>
       </c>
@@ -3569,7 +3564,7 @@
       </c>
       <c r="H132" s="1"/>
     </row>
-    <row r="133" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
         <v>51</v>
       </c>
@@ -3585,7 +3580,7 @@
       </c>
       <c r="H133" s="1"/>
     </row>
-    <row r="134" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
         <v>50</v>
       </c>
@@ -3601,7 +3596,7 @@
       </c>
       <c r="H134" s="1"/>
     </row>
-    <row r="135" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
         <v>49</v>
       </c>
@@ -3617,7 +3612,7 @@
       </c>
       <c r="H135" s="1"/>
     </row>
-    <row r="136" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
         <v>48</v>
       </c>
@@ -3633,7 +3628,7 @@
       </c>
       <c r="H136" s="1"/>
     </row>
-    <row r="137" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
         <v>47</v>
       </c>
@@ -3649,7 +3644,7 @@
       </c>
       <c r="H137" s="1"/>
     </row>
-    <row r="138" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
         <v>46</v>
       </c>
@@ -3665,7 +3660,7 @@
       </c>
       <c r="H138" s="1"/>
     </row>
-    <row r="139" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
         <v>45</v>
       </c>
@@ -3681,7 +3676,7 @@
       </c>
       <c r="H139" s="1"/>
     </row>
-    <row r="140" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
         <v>44</v>
       </c>
@@ -3697,7 +3692,7 @@
       </c>
       <c r="H140" s="1"/>
     </row>
-    <row r="141" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
         <v>43</v>
       </c>
@@ -3713,7 +3708,7 @@
       </c>
       <c r="H141" s="1"/>
     </row>
-    <row r="142" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
         <v>42</v>
       </c>
@@ -3729,7 +3724,7 @@
       </c>
       <c r="H142" s="1"/>
     </row>
-    <row r="143" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
         <v>41</v>
       </c>
@@ -3745,7 +3740,7 @@
       </c>
       <c r="H143" s="1"/>
     </row>
-    <row r="144" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
         <v>40</v>
       </c>
@@ -3761,7 +3756,7 @@
       </c>
       <c r="H144" s="1"/>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
         <v>117</v>
       </c>
@@ -3787,10 +3782,10 @@
         <v>100</v>
       </c>
       <c r="I145" s="2" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="146" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
         <v>38</v>
       </c>
@@ -3806,7 +3801,7 @@
       </c>
       <c r="H146" s="1"/>
     </row>
-    <row r="147" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
         <v>37</v>
       </c>
@@ -3822,7 +3817,7 @@
       </c>
       <c r="H147" s="1"/>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
         <v>108</v>
       </c>
@@ -3848,10 +3843,10 @@
         <v>100</v>
       </c>
       <c r="I148" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="149" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="149" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
         <v>35</v>
       </c>
@@ -3867,7 +3862,7 @@
       </c>
       <c r="H149" s="1"/>
     </row>
-    <row r="150" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
         <v>34</v>
       </c>
@@ -3883,7 +3878,7 @@
       </c>
       <c r="H150" s="1"/>
     </row>
-    <row r="151" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
         <v>33</v>
       </c>
@@ -3899,36 +3894,36 @@
       </c>
       <c r="H151" s="1"/>
     </row>
-    <row r="152" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="5" t="s">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
         <v>195</v>
       </c>
-      <c r="B152" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C152" s="5">
+      <c r="B152" t="s">
+        <v>0</v>
+      </c>
+      <c r="C152">
         <v>390</v>
       </c>
-      <c r="D152" s="6">
-        <v>0</v>
-      </c>
-      <c r="E152" s="5">
+      <c r="D152" s="1">
+        <v>0</v>
+      </c>
+      <c r="E152">
         <v>55</v>
       </c>
-      <c r="F152" s="5">
+      <c r="F152">
         <v>3</v>
       </c>
-      <c r="G152" s="5" t="s">
+      <c r="G152" t="s">
         <v>8</v>
       </c>
-      <c r="H152" s="5">
+      <c r="H152">
         <v>100</v>
       </c>
-      <c r="I152" s="7" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="153" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I152" s="2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="153" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
         <v>31</v>
       </c>
@@ -3944,7 +3939,7 @@
       </c>
       <c r="H153" s="1"/>
     </row>
-    <row r="154" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
         <v>30</v>
       </c>
@@ -3960,7 +3955,7 @@
       </c>
       <c r="H154" s="1"/>
     </row>
-    <row r="155" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
         <v>29</v>
       </c>
@@ -3976,36 +3971,36 @@
       </c>
       <c r="H155" s="1"/>
     </row>
-    <row r="156" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A156" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="B156" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C156" s="5">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
+        <v>200</v>
+      </c>
+      <c r="B156" t="s">
+        <v>0</v>
+      </c>
+      <c r="C156">
         <v>330</v>
       </c>
-      <c r="D156" s="6">
-        <v>0</v>
-      </c>
-      <c r="E156" s="5">
+      <c r="D156" s="1">
+        <v>0</v>
+      </c>
+      <c r="E156">
         <v>50</v>
       </c>
-      <c r="F156" s="5">
-        <v>1</v>
-      </c>
-      <c r="G156" s="5" t="s">
+      <c r="F156">
+        <v>1</v>
+      </c>
+      <c r="G156" t="s">
         <v>8</v>
       </c>
-      <c r="H156" s="5">
+      <c r="H156">
         <v>100</v>
       </c>
-      <c r="I156" s="7" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I156" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
         <v>81</v>
       </c>
@@ -4031,10 +4026,10 @@
         <v>100</v>
       </c>
       <c r="I157" s="2" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="158" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="158" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
         <v>26</v>
       </c>
@@ -4050,7 +4045,7 @@
       </c>
       <c r="H158" s="1"/>
     </row>
-    <row r="159" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
         <v>25</v>
       </c>
@@ -4066,7 +4061,7 @@
       </c>
       <c r="H159" s="1"/>
     </row>
-    <row r="160" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
         <v>24</v>
       </c>
@@ -4082,7 +4077,7 @@
       </c>
       <c r="H160" s="1"/>
     </row>
-    <row r="161" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
         <v>23</v>
       </c>
@@ -4098,7 +4093,7 @@
       </c>
       <c r="H161" s="1"/>
     </row>
-    <row r="162" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
         <v>22</v>
       </c>
@@ -4114,7 +4109,7 @@
       </c>
       <c r="H162" s="1"/>
     </row>
-    <row r="163" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
         <v>21</v>
       </c>
@@ -4130,7 +4125,7 @@
       </c>
       <c r="H163" s="1"/>
     </row>
-    <row r="164" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
         <v>20</v>
       </c>
@@ -4146,7 +4141,7 @@
       </c>
       <c r="H164" s="1"/>
     </row>
-    <row r="165" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
         <v>19</v>
       </c>
@@ -4162,7 +4157,7 @@
       </c>
       <c r="H165" s="1"/>
     </row>
-    <row r="166" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
         <v>18</v>
       </c>
@@ -4178,7 +4173,7 @@
       </c>
       <c r="H166" s="1"/>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
         <v>191</v>
       </c>
@@ -4204,10 +4199,10 @@
         <v>50</v>
       </c>
       <c r="I167" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="168" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="168" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
         <v>16</v>
       </c>
@@ -4223,7 +4218,7 @@
       </c>
       <c r="H168" s="1"/>
     </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
         <v>76</v>
       </c>
@@ -4249,10 +4244,10 @@
         <v>100</v>
       </c>
       <c r="I169" s="2" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="170" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="170" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
         <v>14</v>
       </c>
@@ -4268,7 +4263,7 @@
       </c>
       <c r="H170" s="1"/>
     </row>
-    <row r="171" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
         <v>13</v>
       </c>
@@ -4284,7 +4279,7 @@
       </c>
       <c r="H171" s="1"/>
     </row>
-    <row r="172" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
         <v>12</v>
       </c>
@@ -4300,7 +4295,7 @@
       </c>
       <c r="H172" s="1"/>
     </row>
-    <row r="173" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
         <v>11</v>
       </c>
@@ -4316,7 +4311,7 @@
       </c>
       <c r="H173" s="1"/>
     </row>
-    <row r="174" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
         <v>10</v>
       </c>
@@ -4332,7 +4327,7 @@
       </c>
       <c r="H174" s="1"/>
     </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="s">
         <v>74</v>
       </c>
@@ -4358,10 +4353,10 @@
         <v>100</v>
       </c>
       <c r="I175" s="2" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="176" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="176" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
         <v>7</v>
       </c>
@@ -4377,7 +4372,7 @@
       </c>
       <c r="H176" s="1"/>
     </row>
-    <row r="177" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A177" s="1" t="s">
         <v>6</v>
       </c>
@@ -4393,7 +4388,7 @@
       </c>
       <c r="H177" s="1"/>
     </row>
-    <row r="178" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
         <v>5</v>
       </c>
@@ -4409,7 +4404,7 @@
       </c>
       <c r="H178" s="1"/>
     </row>
-    <row r="179" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
         <v>4</v>
       </c>
@@ -4425,7 +4420,7 @@
       </c>
       <c r="H179" s="1"/>
     </row>
-    <row r="180" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
         <v>3</v>
       </c>
@@ -4441,7 +4436,7 @@
       </c>
       <c r="H180" s="1"/>
     </row>
-    <row r="181" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A181" s="1" t="s">
         <v>2</v>
       </c>
@@ -4457,7 +4452,7 @@
       </c>
       <c r="H181" s="1"/>
     </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A182" s="1" t="s">
         <v>73</v>
       </c>
@@ -4483,39 +4478,39 @@
         <v>100</v>
       </c>
       <c r="I182" s="2" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="183" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A183" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B183" s="5" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="183" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A183" t="s">
+        <v>245</v>
+      </c>
+      <c r="B183" t="s">
         <v>193</v>
       </c>
-      <c r="C183" s="5">
+      <c r="C183">
         <v>350</v>
       </c>
-      <c r="D183" s="6">
-        <v>0</v>
-      </c>
-      <c r="E183" s="5">
+      <c r="D183" s="1">
+        <v>0</v>
+      </c>
+      <c r="E183">
         <v>100</v>
       </c>
-      <c r="F183" s="5">
+      <c r="F183">
         <v>5</v>
       </c>
-      <c r="G183" s="5" t="s">
+      <c r="G183" t="s">
         <v>8</v>
       </c>
-      <c r="H183" s="5">
+      <c r="H183">
         <v>100</v>
       </c>
-      <c r="I183" s="7" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I183" s="2" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="184" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A184" s="1" t="s">
         <v>39</v>
       </c>
@@ -4541,10 +4536,10 @@
         <v>100</v>
       </c>
       <c r="I184" s="2" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="185" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A185" s="1" t="s">
         <v>36</v>
       </c>
@@ -4570,10 +4565,10 @@
         <v>100</v>
       </c>
       <c r="I185" s="3" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="186" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A186" s="1" t="s">
         <v>32</v>
       </c>
@@ -4599,10 +4594,10 @@
         <v>100</v>
       </c>
       <c r="I186" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="187" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A187" s="1" t="s">
         <v>28</v>
       </c>
@@ -4628,210 +4623,210 @@
         <v>100</v>
       </c>
       <c r="I187" s="2" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="188" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A188" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B188" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C188" s="1">
+        <v>500</v>
+      </c>
+      <c r="D188" s="1">
+        <v>0</v>
+      </c>
+      <c r="E188" s="1">
+        <v>200</v>
+      </c>
+      <c r="F188" s="1">
+        <v>5</v>
+      </c>
+      <c r="G188" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H188">
+        <v>100</v>
+      </c>
+      <c r="I188" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="189" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A189" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B189" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C189" s="1">
+        <v>440</v>
+      </c>
+      <c r="D189" s="1">
+        <v>0</v>
+      </c>
+      <c r="E189" s="1">
+        <v>150</v>
+      </c>
+      <c r="F189" s="1">
+        <v>3</v>
+      </c>
+      <c r="G189" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H189">
+        <v>100</v>
+      </c>
+      <c r="I189" s="3" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="188" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A188" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B188" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C188" s="6">
-        <v>500</v>
-      </c>
-      <c r="D188" s="6">
-        <v>0</v>
-      </c>
-      <c r="E188" s="6">
-        <v>200</v>
-      </c>
-      <c r="F188" s="6">
+    <row r="190" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A190" t="s">
+        <v>197</v>
+      </c>
+      <c r="B190" t="s">
+        <v>0</v>
+      </c>
+      <c r="C190">
+        <v>400</v>
+      </c>
+      <c r="D190" s="1">
+        <v>0</v>
+      </c>
+      <c r="E190">
+        <v>55</v>
+      </c>
+      <c r="F190">
+        <v>1</v>
+      </c>
+      <c r="G190" t="s">
+        <v>8</v>
+      </c>
+      <c r="H190">
+        <v>100</v>
+      </c>
+      <c r="I190" s="2" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="191" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A191" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B191" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C191" s="1">
+        <v>440</v>
+      </c>
+      <c r="D191" s="1">
+        <v>0</v>
+      </c>
+      <c r="E191">
+        <v>55</v>
+      </c>
+      <c r="F191">
         <v>5</v>
       </c>
-      <c r="G188" s="6" t="s">
+      <c r="G191" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H188" s="5">
+      <c r="H191">
         <v>100</v>
       </c>
-      <c r="I188" s="8" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="189" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A189" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B189" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C189" s="6">
-        <v>440</v>
-      </c>
-      <c r="D189" s="6">
-        <v>0</v>
-      </c>
-      <c r="E189" s="6">
+      <c r="I191" s="2" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="192" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A192" t="s">
+        <v>199</v>
+      </c>
+      <c r="B192" t="s">
+        <v>0</v>
+      </c>
+      <c r="C192">
+        <v>370</v>
+      </c>
+      <c r="D192" s="1">
+        <v>0</v>
+      </c>
+      <c r="E192">
         <v>150</v>
       </c>
-      <c r="F189" s="6">
+      <c r="F192">
+        <v>0</v>
+      </c>
+      <c r="G192" t="s">
+        <v>8</v>
+      </c>
+      <c r="H192">
+        <v>100</v>
+      </c>
+      <c r="I192" s="2" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="193" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A193" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B193" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C193">
+        <v>390</v>
+      </c>
+      <c r="D193" s="1">
+        <v>0</v>
+      </c>
+      <c r="E193" s="1">
+        <v>165</v>
+      </c>
+      <c r="F193" s="1">
+        <v>10</v>
+      </c>
+      <c r="G193" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H193">
+        <v>100</v>
+      </c>
+      <c r="I193" s="2" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="194" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A194" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B194" t="s">
+        <v>193</v>
+      </c>
+      <c r="C194" s="1">
+        <v>510</v>
+      </c>
+      <c r="D194" s="1">
+        <v>0</v>
+      </c>
+      <c r="E194" s="1">
+        <v>70</v>
+      </c>
+      <c r="F194" s="1">
         <v>3</v>
       </c>
-      <c r="G189" s="6" t="s">
+      <c r="G194" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H189" s="5">
+      <c r="H194">
         <v>100</v>
       </c>
-      <c r="I189" s="8" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="190" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A190" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="B190" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C190" s="5">
-        <v>400</v>
-      </c>
-      <c r="D190" s="6">
-        <v>0</v>
-      </c>
-      <c r="E190" s="5">
-        <v>55</v>
-      </c>
-      <c r="F190" s="5">
-        <v>1</v>
-      </c>
-      <c r="G190" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H190" s="5">
-        <v>100</v>
-      </c>
-      <c r="I190" s="7" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="191" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A191" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B191" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C191" s="6">
-        <v>440</v>
-      </c>
-      <c r="D191" s="6">
-        <v>0</v>
-      </c>
-      <c r="E191" s="5">
-        <v>55</v>
-      </c>
-      <c r="F191" s="5">
-        <v>5</v>
-      </c>
-      <c r="G191" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H191" s="5">
-        <v>100</v>
-      </c>
-      <c r="I191" s="7" t="s">
+      <c r="I194" s="2" t="s">
         <v>242</v>
-      </c>
-    </row>
-    <row r="192" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A192" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="B192" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C192" s="5">
-        <v>370</v>
-      </c>
-      <c r="D192" s="6">
-        <v>0</v>
-      </c>
-      <c r="E192" s="5">
-        <v>150</v>
-      </c>
-      <c r="F192" s="5">
-        <v>0</v>
-      </c>
-      <c r="G192" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H192" s="5">
-        <v>100</v>
-      </c>
-      <c r="I192" s="7" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="193" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A193" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B193" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C193" s="5">
-        <v>390</v>
-      </c>
-      <c r="D193" s="6">
-        <v>0</v>
-      </c>
-      <c r="E193" s="6">
-        <v>165</v>
-      </c>
-      <c r="F193" s="6">
-        <v>10</v>
-      </c>
-      <c r="G193" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H193" s="5">
-        <v>100</v>
-      </c>
-      <c r="I193" s="7" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="194" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A194" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="B194" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="C194" s="6">
-        <v>510</v>
-      </c>
-      <c r="D194" s="6">
-        <v>0</v>
-      </c>
-      <c r="E194" s="6">
-        <v>70</v>
-      </c>
-      <c r="F194" s="6">
-        <v>3</v>
-      </c>
-      <c r="G194" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H194" s="5">
-        <v>100</v>
-      </c>
-      <c r="I194" s="7" t="s">
-        <v>244</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
leads before and after 1 april
Column with leads after 1 april added, but not tested yet
</commit_message>
<xml_diff>
--- a/templates/programs.xlsx
+++ b/templates/programs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/iasonov/Programming/Python/HSE_dashboard/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tijuanap\Programs\HSE_dashboard\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA7389B3-0AF7-BA45-8B59-8075E4564235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AEF04B2-0459-43BE-B2B7-E378E95958C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16460" xr2:uid="{459C6DFD-26EB-1040-9D7C-59DC53018D97}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{459C6DFD-26EB-1040-9D7C-59DC53018D97}"/>
   </bookViews>
   <sheets>
     <sheet name="programs" sheetId="1" r:id="rId1"/>
@@ -873,9 +873,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -913,7 +913,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1019,7 +1019,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1161,7 +1161,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1172,20 +1172,20 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:I194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="150" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I77" sqref="I77"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I194" sqref="A1:I194"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.83203125" customWidth="1"/>
-    <col min="2" max="2" width="8.1640625" customWidth="1"/>
-    <col min="3" max="6" width="7.6640625" customWidth="1"/>
+    <col min="1" max="1" width="35.875" customWidth="1"/>
+    <col min="2" max="2" width="8.125" customWidth="1"/>
+    <col min="3" max="6" width="7.625" customWidth="1"/>
     <col min="8" max="8" width="6" customWidth="1"/>
     <col min="9" max="9" width="46" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>185</v>
       </c>
@@ -1214,7 +1214,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="2" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>183</v>
       </c>
@@ -1230,7 +1230,7 @@
       </c>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>182</v>
       </c>
@@ -1246,7 +1246,7 @@
       </c>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>181</v>
       </c>
@@ -1262,7 +1262,7 @@
       </c>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>180</v>
       </c>
@@ -1278,7 +1278,7 @@
       </c>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>179</v>
       </c>
@@ -1294,7 +1294,7 @@
       </c>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>178</v>
       </c>
@@ -1310,7 +1310,7 @@
       </c>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>177</v>
       </c>
@@ -1339,7 +1339,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>176</v>
       </c>
@@ -1355,7 +1355,7 @@
       </c>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>175</v>
       </c>
@@ -1384,7 +1384,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>174</v>
       </c>
@@ -1400,7 +1400,7 @@
       </c>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>173</v>
       </c>
@@ -1416,7 +1416,7 @@
       </c>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>172</v>
       </c>
@@ -1432,7 +1432,7 @@
       </c>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>171</v>
       </c>
@@ -1448,7 +1448,7 @@
       </c>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>170</v>
       </c>
@@ -1464,7 +1464,7 @@
       </c>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>169</v>
       </c>
@@ -1480,7 +1480,7 @@
       </c>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>168</v>
       </c>
@@ -1496,7 +1496,7 @@
       </c>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>167</v>
       </c>
@@ -1512,7 +1512,7 @@
       </c>
       <c r="H18" s="1"/>
     </row>
-    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>166</v>
       </c>
@@ -1528,7 +1528,7 @@
       </c>
       <c r="H19" s="1"/>
     </row>
-    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>165</v>
       </c>
@@ -1544,7 +1544,7 @@
       </c>
       <c r="H20" s="1"/>
     </row>
-    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>164</v>
       </c>
@@ -1560,7 +1560,7 @@
       </c>
       <c r="H21" s="1"/>
     </row>
-    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>163</v>
       </c>
@@ -1576,7 +1576,7 @@
       </c>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>162</v>
       </c>
@@ -1592,7 +1592,7 @@
       </c>
       <c r="H23" s="1"/>
     </row>
-    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>161</v>
       </c>
@@ -1608,7 +1608,7 @@
       </c>
       <c r="H24" s="1"/>
     </row>
-    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>160</v>
       </c>
@@ -1624,7 +1624,7 @@
       </c>
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>159</v>
       </c>
@@ -1640,7 +1640,7 @@
       </c>
       <c r="H26" s="1"/>
     </row>
-    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>158</v>
       </c>
@@ -1656,7 +1656,7 @@
       </c>
       <c r="H27" s="1"/>
     </row>
-    <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>157</v>
       </c>
@@ -1672,7 +1672,7 @@
       </c>
       <c r="H28" s="1"/>
     </row>
-    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>156</v>
       </c>
@@ -1688,7 +1688,7 @@
       </c>
       <c r="H29" s="1"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>198</v>
       </c>
@@ -1717,7 +1717,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>187</v>
       </c>
@@ -1746,7 +1746,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>153</v>
       </c>
@@ -1762,7 +1762,7 @@
       </c>
       <c r="H32" s="1"/>
     </row>
-    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>152</v>
       </c>
@@ -1778,7 +1778,7 @@
       </c>
       <c r="H33" s="1"/>
     </row>
-    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>151</v>
       </c>
@@ -1794,7 +1794,7 @@
       </c>
       <c r="H34" s="1"/>
     </row>
-    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>150</v>
       </c>
@@ -1810,7 +1810,7 @@
       </c>
       <c r="H35" s="1"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>188</v>
       </c>
@@ -1839,7 +1839,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>148</v>
       </c>
@@ -1855,7 +1855,7 @@
       </c>
       <c r="H37" s="1"/>
     </row>
-    <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>147</v>
       </c>
@@ -1871,7 +1871,7 @@
       </c>
       <c r="H38" s="1"/>
     </row>
-    <row r="39" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>146</v>
       </c>
@@ -1887,7 +1887,7 @@
       </c>
       <c r="H39" s="1"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>189</v>
       </c>
@@ -1916,7 +1916,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>155</v>
       </c>
@@ -1945,7 +1945,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>154</v>
       </c>
@@ -1974,7 +1974,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="43" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>142</v>
       </c>
@@ -1990,7 +1990,7 @@
       </c>
       <c r="H43" s="1"/>
     </row>
-    <row r="44" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>141</v>
       </c>
@@ -2006,7 +2006,7 @@
       </c>
       <c r="H44" s="1"/>
     </row>
-    <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>140</v>
       </c>
@@ -2022,7 +2022,7 @@
       </c>
       <c r="H45" s="1"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>149</v>
       </c>
@@ -2051,7 +2051,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>145</v>
       </c>
@@ -2080,7 +2080,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="48" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>137</v>
       </c>
@@ -2096,7 +2096,7 @@
       </c>
       <c r="H48" s="1"/>
     </row>
-    <row r="49" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>136</v>
       </c>
@@ -2112,7 +2112,7 @@
       </c>
       <c r="H49" s="1"/>
     </row>
-    <row r="50" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>135</v>
       </c>
@@ -2128,7 +2128,7 @@
       </c>
       <c r="H50" s="1"/>
     </row>
-    <row r="51" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>134</v>
       </c>
@@ -2144,7 +2144,7 @@
       </c>
       <c r="H51" s="1"/>
     </row>
-    <row r="52" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>133</v>
       </c>
@@ -2160,7 +2160,7 @@
       </c>
       <c r="H52" s="1"/>
     </row>
-    <row r="53" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>132</v>
       </c>
@@ -2183,7 +2183,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="54" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>131</v>
       </c>
@@ -2199,7 +2199,7 @@
       </c>
       <c r="H54" s="1"/>
     </row>
-    <row r="55" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>130</v>
       </c>
@@ -2215,7 +2215,7 @@
       </c>
       <c r="H55" s="1"/>
     </row>
-    <row r="56" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>129</v>
       </c>
@@ -2231,7 +2231,7 @@
       </c>
       <c r="H56" s="1"/>
     </row>
-    <row r="57" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>128</v>
       </c>
@@ -2247,7 +2247,7 @@
       </c>
       <c r="H57" s="1"/>
     </row>
-    <row r="58" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>127</v>
       </c>
@@ -2263,7 +2263,7 @@
       </c>
       <c r="H58" s="1"/>
     </row>
-    <row r="59" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>126</v>
       </c>
@@ -2279,7 +2279,7 @@
       </c>
       <c r="H59" s="1"/>
     </row>
-    <row r="60" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>125</v>
       </c>
@@ -2295,7 +2295,7 @@
       </c>
       <c r="H60" s="1"/>
     </row>
-    <row r="61" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>124</v>
       </c>
@@ -2311,7 +2311,7 @@
       </c>
       <c r="H61" s="1"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>144</v>
       </c>
@@ -2340,7 +2340,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="63" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>122</v>
       </c>
@@ -2356,7 +2356,7 @@
       </c>
       <c r="H63" s="1"/>
     </row>
-    <row r="64" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>121</v>
       </c>
@@ -2372,7 +2372,7 @@
       </c>
       <c r="H64" s="1"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>143</v>
       </c>
@@ -2401,7 +2401,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>139</v>
       </c>
@@ -2430,7 +2430,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="67" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>118</v>
       </c>
@@ -2446,7 +2446,7 @@
       </c>
       <c r="H67" s="1"/>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>138</v>
       </c>
@@ -2475,7 +2475,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="69" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>116</v>
       </c>
@@ -2491,7 +2491,7 @@
       </c>
       <c r="H69" s="1"/>
     </row>
-    <row r="70" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>115</v>
       </c>
@@ -2507,7 +2507,7 @@
       </c>
       <c r="H70" s="1"/>
     </row>
-    <row r="71" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>114</v>
       </c>
@@ -2523,7 +2523,7 @@
       </c>
       <c r="H71" s="1"/>
     </row>
-    <row r="72" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>113</v>
       </c>
@@ -2539,7 +2539,7 @@
       </c>
       <c r="H72" s="1"/>
     </row>
-    <row r="73" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>112</v>
       </c>
@@ -2555,7 +2555,7 @@
       </c>
       <c r="H73" s="1"/>
     </row>
-    <row r="74" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>111</v>
       </c>
@@ -2571,7 +2571,7 @@
       </c>
       <c r="H74" s="1"/>
     </row>
-    <row r="75" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>110</v>
       </c>
@@ -2587,7 +2587,7 @@
       </c>
       <c r="H75" s="1"/>
     </row>
-    <row r="76" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>109</v>
       </c>
@@ -2603,7 +2603,7 @@
       </c>
       <c r="H76" s="1"/>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>196</v>
       </c>
@@ -2632,7 +2632,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="78" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>107</v>
       </c>
@@ -2648,7 +2648,7 @@
       </c>
       <c r="H78" s="1"/>
     </row>
-    <row r="79" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>106</v>
       </c>
@@ -2664,7 +2664,7 @@
       </c>
       <c r="H79" s="1"/>
     </row>
-    <row r="80" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>105</v>
       </c>
@@ -2680,7 +2680,7 @@
       </c>
       <c r="H80" s="1"/>
     </row>
-    <row r="81" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>104</v>
       </c>
@@ -2696,7 +2696,7 @@
       </c>
       <c r="H81" s="1"/>
     </row>
-    <row r="82" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>103</v>
       </c>
@@ -2712,7 +2712,7 @@
       </c>
       <c r="H82" s="1"/>
     </row>
-    <row r="83" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>102</v>
       </c>
@@ -2728,7 +2728,7 @@
       </c>
       <c r="H83" s="1"/>
     </row>
-    <row r="84" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>101</v>
       </c>
@@ -2744,7 +2744,7 @@
       </c>
       <c r="H84" s="1"/>
     </row>
-    <row r="85" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>100</v>
       </c>
@@ -2760,7 +2760,7 @@
       </c>
       <c r="H85" s="1"/>
     </row>
-    <row r="86" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>99</v>
       </c>
@@ -2776,7 +2776,7 @@
       </c>
       <c r="H86" s="1"/>
     </row>
-    <row r="87" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>98</v>
       </c>
@@ -2792,7 +2792,7 @@
       </c>
       <c r="H87" s="1"/>
     </row>
-    <row r="88" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>97</v>
       </c>
@@ -2808,7 +2808,7 @@
       </c>
       <c r="H88" s="1"/>
     </row>
-    <row r="89" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>96</v>
       </c>
@@ -2824,7 +2824,7 @@
       </c>
       <c r="H89" s="1"/>
     </row>
-    <row r="90" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>95</v>
       </c>
@@ -2840,7 +2840,7 @@
       </c>
       <c r="H90" s="1"/>
     </row>
-    <row r="91" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>94</v>
       </c>
@@ -2856,7 +2856,7 @@
       </c>
       <c r="H91" s="1"/>
     </row>
-    <row r="92" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>93</v>
       </c>
@@ -2872,7 +2872,7 @@
       </c>
       <c r="H92" s="1"/>
     </row>
-    <row r="93" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>92</v>
       </c>
@@ -2888,7 +2888,7 @@
       </c>
       <c r="H93" s="1"/>
     </row>
-    <row r="94" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>91</v>
       </c>
@@ -2904,7 +2904,7 @@
       </c>
       <c r="H94" s="1"/>
     </row>
-    <row r="95" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>90</v>
       </c>
@@ -2920,7 +2920,7 @@
       </c>
       <c r="H95" s="1"/>
     </row>
-    <row r="96" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>89</v>
       </c>
@@ -2936,7 +2936,7 @@
       </c>
       <c r="H96" s="1"/>
     </row>
-    <row r="97" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>88</v>
       </c>
@@ -2952,7 +2952,7 @@
       </c>
       <c r="H97" s="1"/>
     </row>
-    <row r="98" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>87</v>
       </c>
@@ -2968,7 +2968,7 @@
       </c>
       <c r="H98" s="1"/>
     </row>
-    <row r="99" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>86</v>
       </c>
@@ -2984,7 +2984,7 @@
       </c>
       <c r="H99" s="1"/>
     </row>
-    <row r="100" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>85</v>
       </c>
@@ -3000,7 +3000,7 @@
       </c>
       <c r="H100" s="1"/>
     </row>
-    <row r="101" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>84</v>
       </c>
@@ -3016,7 +3016,7 @@
       </c>
       <c r="H101" s="1"/>
     </row>
-    <row r="102" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>83</v>
       </c>
@@ -3032,7 +3032,7 @@
       </c>
       <c r="H102" s="1"/>
     </row>
-    <row r="103" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>82</v>
       </c>
@@ -3048,7 +3048,7 @@
       </c>
       <c r="H103" s="1"/>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>190</v>
       </c>
@@ -3077,7 +3077,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="105" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>80</v>
       </c>
@@ -3093,7 +3093,7 @@
       </c>
       <c r="H105" s="1"/>
     </row>
-    <row r="106" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>79</v>
       </c>
@@ -3109,7 +3109,7 @@
       </c>
       <c r="H106" s="1"/>
     </row>
-    <row r="107" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>78</v>
       </c>
@@ -3125,7 +3125,7 @@
       </c>
       <c r="H107" s="1"/>
     </row>
-    <row r="108" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>77</v>
       </c>
@@ -3141,7 +3141,7 @@
       </c>
       <c r="H108" s="1"/>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>123</v>
       </c>
@@ -3170,7 +3170,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="110" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>75</v>
       </c>
@@ -3186,7 +3186,7 @@
       </c>
       <c r="H110" s="1"/>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>120</v>
       </c>
@@ -3215,7 +3215,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>119</v>
       </c>
@@ -3244,7 +3244,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="113" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>71</v>
       </c>
@@ -3260,7 +3260,7 @@
       </c>
       <c r="H113" s="1"/>
     </row>
-    <row r="114" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>70</v>
       </c>
@@ -3276,7 +3276,7 @@
       </c>
       <c r="H114" s="1"/>
     </row>
-    <row r="115" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>69</v>
       </c>
@@ -3292,7 +3292,7 @@
       </c>
       <c r="H115" s="1"/>
     </row>
-    <row r="116" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>68</v>
       </c>
@@ -3308,7 +3308,7 @@
       </c>
       <c r="H116" s="1"/>
     </row>
-    <row r="117" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>67</v>
       </c>
@@ -3324,7 +3324,7 @@
       </c>
       <c r="H117" s="1"/>
     </row>
-    <row r="118" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>66</v>
       </c>
@@ -3340,7 +3340,7 @@
       </c>
       <c r="H118" s="1"/>
     </row>
-    <row r="119" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>65</v>
       </c>
@@ -3356,7 +3356,7 @@
       </c>
       <c r="H119" s="1"/>
     </row>
-    <row r="120" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>64</v>
       </c>
@@ -3372,7 +3372,7 @@
       </c>
       <c r="H120" s="1"/>
     </row>
-    <row r="121" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>63</v>
       </c>
@@ -3388,7 +3388,7 @@
       </c>
       <c r="H121" s="1"/>
     </row>
-    <row r="122" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>62</v>
       </c>
@@ -3404,7 +3404,7 @@
       </c>
       <c r="H122" s="1"/>
     </row>
-    <row r="123" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>61</v>
       </c>
@@ -3420,7 +3420,7 @@
       </c>
       <c r="H123" s="1"/>
     </row>
-    <row r="124" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>60</v>
       </c>
@@ -3436,7 +3436,7 @@
       </c>
       <c r="H124" s="1"/>
     </row>
-    <row r="125" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>59</v>
       </c>
@@ -3452,7 +3452,7 @@
       </c>
       <c r="H125" s="1"/>
     </row>
-    <row r="126" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>58</v>
       </c>
@@ -3468,7 +3468,7 @@
       </c>
       <c r="H126" s="1"/>
     </row>
-    <row r="127" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>57</v>
       </c>
@@ -3484,7 +3484,7 @@
       </c>
       <c r="H127" s="1"/>
     </row>
-    <row r="128" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>56</v>
       </c>
@@ -3500,7 +3500,7 @@
       </c>
       <c r="H128" s="1"/>
     </row>
-    <row r="129" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>55</v>
       </c>
@@ -3516,7 +3516,7 @@
       </c>
       <c r="H129" s="1"/>
     </row>
-    <row r="130" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>54</v>
       </c>
@@ -3532,7 +3532,7 @@
       </c>
       <c r="H130" s="1"/>
     </row>
-    <row r="131" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>53</v>
       </c>
@@ -3548,7 +3548,7 @@
       </c>
       <c r="H131" s="1"/>
     </row>
-    <row r="132" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>52</v>
       </c>
@@ -3564,7 +3564,7 @@
       </c>
       <c r="H132" s="1"/>
     </row>
-    <row r="133" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>51</v>
       </c>
@@ -3580,7 +3580,7 @@
       </c>
       <c r="H133" s="1"/>
     </row>
-    <row r="134" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>50</v>
       </c>
@@ -3596,7 +3596,7 @@
       </c>
       <c r="H134" s="1"/>
     </row>
-    <row r="135" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>49</v>
       </c>
@@ -3612,7 +3612,7 @@
       </c>
       <c r="H135" s="1"/>
     </row>
-    <row r="136" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>48</v>
       </c>
@@ -3628,7 +3628,7 @@
       </c>
       <c r="H136" s="1"/>
     </row>
-    <row r="137" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>47</v>
       </c>
@@ -3644,7 +3644,7 @@
       </c>
       <c r="H137" s="1"/>
     </row>
-    <row r="138" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>46</v>
       </c>
@@ -3660,7 +3660,7 @@
       </c>
       <c r="H138" s="1"/>
     </row>
-    <row r="139" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>45</v>
       </c>
@@ -3676,7 +3676,7 @@
       </c>
       <c r="H139" s="1"/>
     </row>
-    <row r="140" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>44</v>
       </c>
@@ -3692,7 +3692,7 @@
       </c>
       <c r="H140" s="1"/>
     </row>
-    <row r="141" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
         <v>43</v>
       </c>
@@ -3708,7 +3708,7 @@
       </c>
       <c r="H141" s="1"/>
     </row>
-    <row r="142" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>42</v>
       </c>
@@ -3724,7 +3724,7 @@
       </c>
       <c r="H142" s="1"/>
     </row>
-    <row r="143" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>41</v>
       </c>
@@ -3740,7 +3740,7 @@
       </c>
       <c r="H143" s="1"/>
     </row>
-    <row r="144" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>40</v>
       </c>
@@ -3756,7 +3756,7 @@
       </c>
       <c r="H144" s="1"/>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
         <v>117</v>
       </c>
@@ -3785,7 +3785,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="146" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>38</v>
       </c>
@@ -3801,7 +3801,7 @@
       </c>
       <c r="H146" s="1"/>
     </row>
-    <row r="147" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
         <v>37</v>
       </c>
@@ -3817,7 +3817,7 @@
       </c>
       <c r="H147" s="1"/>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
         <v>108</v>
       </c>
@@ -3846,7 +3846,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="149" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
         <v>35</v>
       </c>
@@ -3862,7 +3862,7 @@
       </c>
       <c r="H149" s="1"/>
     </row>
-    <row r="150" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
         <v>34</v>
       </c>
@@ -3878,7 +3878,7 @@
       </c>
       <c r="H150" s="1"/>
     </row>
-    <row r="151" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
         <v>33</v>
       </c>
@@ -3894,7 +3894,7 @@
       </c>
       <c r="H151" s="1"/>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>195</v>
       </c>
@@ -3923,7 +3923,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="153" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
         <v>31</v>
       </c>
@@ -3939,7 +3939,7 @@
       </c>
       <c r="H153" s="1"/>
     </row>
-    <row r="154" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
         <v>30</v>
       </c>
@@ -3955,7 +3955,7 @@
       </c>
       <c r="H154" s="1"/>
     </row>
-    <row r="155" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
         <v>29</v>
       </c>
@@ -3971,7 +3971,7 @@
       </c>
       <c r="H155" s="1"/>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>200</v>
       </c>
@@ -4000,7 +4000,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
         <v>81</v>
       </c>
@@ -4029,7 +4029,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="158" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>26</v>
       </c>
@@ -4045,7 +4045,7 @@
       </c>
       <c r="H158" s="1"/>
     </row>
-    <row r="159" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
         <v>25</v>
       </c>
@@ -4061,7 +4061,7 @@
       </c>
       <c r="H159" s="1"/>
     </row>
-    <row r="160" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>24</v>
       </c>
@@ -4077,7 +4077,7 @@
       </c>
       <c r="H160" s="1"/>
     </row>
-    <row r="161" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>23</v>
       </c>
@@ -4093,7 +4093,7 @@
       </c>
       <c r="H161" s="1"/>
     </row>
-    <row r="162" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>22</v>
       </c>
@@ -4109,7 +4109,7 @@
       </c>
       <c r="H162" s="1"/>
     </row>
-    <row r="163" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
         <v>21</v>
       </c>
@@ -4125,7 +4125,7 @@
       </c>
       <c r="H163" s="1"/>
     </row>
-    <row r="164" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>20</v>
       </c>
@@ -4141,7 +4141,7 @@
       </c>
       <c r="H164" s="1"/>
     </row>
-    <row r="165" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>19</v>
       </c>
@@ -4157,7 +4157,7 @@
       </c>
       <c r="H165" s="1"/>
     </row>
-    <row r="166" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>18</v>
       </c>
@@ -4173,7 +4173,7 @@
       </c>
       <c r="H166" s="1"/>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
         <v>191</v>
       </c>
@@ -4202,7 +4202,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="168" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
         <v>16</v>
       </c>
@@ -4218,7 +4218,7 @@
       </c>
       <c r="H168" s="1"/>
     </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
         <v>76</v>
       </c>
@@ -4247,7 +4247,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="170" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
         <v>14</v>
       </c>
@@ -4263,7 +4263,7 @@
       </c>
       <c r="H170" s="1"/>
     </row>
-    <row r="171" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
         <v>13</v>
       </c>
@@ -4279,7 +4279,7 @@
       </c>
       <c r="H171" s="1"/>
     </row>
-    <row r="172" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
         <v>12</v>
       </c>
@@ -4295,7 +4295,7 @@
       </c>
       <c r="H172" s="1"/>
     </row>
-    <row r="173" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
         <v>11</v>
       </c>
@@ -4311,7 +4311,7 @@
       </c>
       <c r="H173" s="1"/>
     </row>
-    <row r="174" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
         <v>10</v>
       </c>
@@ -4327,7 +4327,7 @@
       </c>
       <c r="H174" s="1"/>
     </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
         <v>74</v>
       </c>
@@ -4356,7 +4356,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="176" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
         <v>7</v>
       </c>
@@ -4372,7 +4372,7 @@
       </c>
       <c r="H176" s="1"/>
     </row>
-    <row r="177" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
         <v>6</v>
       </c>
@@ -4388,7 +4388,7 @@
       </c>
       <c r="H177" s="1"/>
     </row>
-    <row r="178" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
         <v>5</v>
       </c>
@@ -4404,7 +4404,7 @@
       </c>
       <c r="H178" s="1"/>
     </row>
-    <row r="179" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
         <v>4</v>
       </c>
@@ -4420,7 +4420,7 @@
       </c>
       <c r="H179" s="1"/>
     </row>
-    <row r="180" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
         <v>3</v>
       </c>
@@ -4436,7 +4436,7 @@
       </c>
       <c r="H180" s="1"/>
     </row>
-    <row r="181" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
         <v>2</v>
       </c>
@@ -4452,7 +4452,7 @@
       </c>
       <c r="H181" s="1"/>
     </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
         <v>73</v>
       </c>
@@ -4481,7 +4481,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>245</v>
       </c>
@@ -4510,7 +4510,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
         <v>39</v>
       </c>
@@ -4539,7 +4539,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
         <v>36</v>
       </c>
@@ -4568,7 +4568,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
         <v>32</v>
       </c>
@@ -4597,7 +4597,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
         <v>28</v>
       </c>
@@ -4626,7 +4626,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
         <v>27</v>
       </c>
@@ -4655,7 +4655,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
         <v>17</v>
       </c>
@@ -4684,7 +4684,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>197</v>
       </c>
@@ -4713,7 +4713,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
         <v>15</v>
       </c>
@@ -4742,7 +4742,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>199</v>
       </c>
@@ -4771,7 +4771,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
         <v>9</v>
       </c>
@@ -4800,7 +4800,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
         <v>192</v>
       </c>

</xml_diff>

<commit_message>
30 to 45% prediction
</commit_message>
<xml_diff>
--- a/templates/programs.xlsx
+++ b/templates/programs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/iasonov/Programming/Python/HSE_dashboard/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5BFEF8E-54DA-D54F-92B4-E9B1FAF57E41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAD95D79-2EED-0443-9576-82DDBCFD1D9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="500" windowWidth="14400" windowHeight="16460" xr2:uid="{459C6DFD-26EB-1040-9D7C-59DC53018D97}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16460" xr2:uid="{459C6DFD-26EB-1040-9D7C-59DC53018D97}"/>
   </bookViews>
   <sheets>
     <sheet name="programs" sheetId="1" r:id="rId1"/>
@@ -718,9 +718,6 @@
     <t>ПЕДДИЗ. Педагогический дизайн теория и практика обучения / Москва / 440401 Педагогическое образование / Институт образования / Магистратура</t>
   </si>
   <si>
-    <t>ПРИКЛИНГ. Прикладная лингвистика обучение иностранному языку и перевод в цифровой среде / НИУ ВШЭ СанктПетербург / 450403 Фундаментальная и прикладная лингвистика / Факультет СанктПетербургская школа гуманитарных наук и искусств / Магистратура</t>
-  </si>
-  <si>
     <t>ПСП. Прикладная социальная психология / Москва / 370401 Психология / факультет социальных наук / Магистратура</t>
   </si>
   <si>
@@ -779,6 +776,9 @@
   </si>
   <si>
     <t>БАКЭКАН. Экономический анализ / Москва / 380301 Экономика / факультет экономических наук / Бакалавриат</t>
+  </si>
+  <si>
+    <t>ПРИКЛИНГ.Прикладная лингвистика обучение иностранному языку и перевод в цифровой среде / НИУ ВШЭ СанктПетербург / 450403 Фундаментальная и прикладная лингвистика / Факультет СанктПетербургская школа гуманитарных наук и искусств / Магистратура</t>
   </si>
 </sst>
 </file>
@@ -1173,7 +1173,7 @@
   <dimension ref="A1:I194"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+      <selection activeCell="I157" sqref="I157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1196,7 +1196,7 @@
         <v>194</v>
       </c>
       <c r="D1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>202</v>
@@ -2629,7 +2629,7 @@
         <v>100</v>
       </c>
       <c r="I77" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="78" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
@@ -3997,7 +3997,7 @@
         <v>100</v>
       </c>
       <c r="I156" s="2" t="s">
-        <v>226</v>
+        <v>246</v>
       </c>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.2">
@@ -4026,7 +4026,7 @@
         <v>100</v>
       </c>
       <c r="I157" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="158" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
@@ -4199,7 +4199,7 @@
         <v>50</v>
       </c>
       <c r="I167" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="168" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
@@ -4244,7 +4244,7 @@
         <v>100</v>
       </c>
       <c r="I169" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="170" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
@@ -4353,7 +4353,7 @@
         <v>100</v>
       </c>
       <c r="I175" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="176" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
@@ -4478,12 +4478,12 @@
         <v>100</v>
       </c>
       <c r="I182" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="183" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B183" t="s">
         <v>193</v>
@@ -4507,7 +4507,7 @@
         <v>100</v>
       </c>
       <c r="I183" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="184" spans="1:9" x14ac:dyDescent="0.2">
@@ -4536,7 +4536,7 @@
         <v>100</v>
       </c>
       <c r="I184" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="185" spans="1:9" x14ac:dyDescent="0.2">
@@ -4565,7 +4565,7 @@
         <v>100</v>
       </c>
       <c r="I185" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="186" spans="1:9" x14ac:dyDescent="0.2">
@@ -4594,7 +4594,7 @@
         <v>100</v>
       </c>
       <c r="I186" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="187" spans="1:9" x14ac:dyDescent="0.2">
@@ -4623,7 +4623,7 @@
         <v>100</v>
       </c>
       <c r="I187" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="188" spans="1:9" x14ac:dyDescent="0.2">
@@ -4652,7 +4652,7 @@
         <v>100</v>
       </c>
       <c r="I188" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="189" spans="1:9" x14ac:dyDescent="0.2">
@@ -4681,7 +4681,7 @@
         <v>100</v>
       </c>
       <c r="I189" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="190" spans="1:9" x14ac:dyDescent="0.2">
@@ -4710,7 +4710,7 @@
         <v>100</v>
       </c>
       <c r="I190" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="191" spans="1:9" x14ac:dyDescent="0.2">
@@ -4739,7 +4739,7 @@
         <v>100</v>
       </c>
       <c r="I191" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="192" spans="1:9" x14ac:dyDescent="0.2">
@@ -4768,7 +4768,7 @@
         <v>100</v>
       </c>
       <c r="I192" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="193" spans="1:9" x14ac:dyDescent="0.2">
@@ -4797,7 +4797,7 @@
         <v>100</v>
       </c>
       <c r="I193" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="194" spans="1:9" x14ac:dyDescent="0.2">
@@ -4826,7 +4826,7 @@
         <v>100</v>
       </c>
       <c r="I194" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Early invitation seems calculated from excel file
</commit_message>
<xml_diff>
--- a/templates/programs.xlsx
+++ b/templates/programs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/iasonov/Programming/Python/HSE_dashboard/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAD95D79-2EED-0443-9576-82DDBCFD1D9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70A80383-A464-5640-B2ED-FE719EF9E684}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16460" xr2:uid="{459C6DFD-26EB-1040-9D7C-59DC53018D97}"/>
+    <workbookView xWindow="3380" yWindow="620" windowWidth="29760" windowHeight="19860" xr2:uid="{459C6DFD-26EB-1040-9D7C-59DC53018D97}"/>
   </bookViews>
   <sheets>
     <sheet name="programs" sheetId="1" r:id="rId1"/>
@@ -1173,7 +1173,7 @@
   <dimension ref="A1:I194"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I157" sqref="I157"/>
+      <selection sqref="A1:I194"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>